<commit_message>
add free proxy maker
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="152">
   <si>
     <t>Last name</t>
   </si>
@@ -427,6 +427,51 @@
   </si>
   <si>
     <t>U20452945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evran </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latife </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmet </t>
+  </si>
+  <si>
+    <t>Vize</t>
+  </si>
+  <si>
+    <t>D12790130</t>
+  </si>
+  <si>
+    <t>birsenaltan1@hotmail.com</t>
+  </si>
+  <si>
+    <t>Karademir</t>
+  </si>
+  <si>
+    <t>MuhammedSalih</t>
+  </si>
+  <si>
+    <t>Sakarya</t>
+  </si>
+  <si>
+    <t>Selver</t>
+  </si>
+  <si>
+    <t>U31185115</t>
+  </si>
+  <si>
+    <t>salihkarademir17@gmail.com</t>
+  </si>
+  <si>
+    <t>1969-04-30</t>
+  </si>
+  <si>
+    <t>1997-28-12</t>
   </si>
 </sst>
 </file>
@@ -485,11 +530,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -791,15 +837,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
@@ -1301,8 +1349,61 @@
         <v>136</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>